<commit_message>
Update Generic Excel DataLayer (iPasXL)
</commit_message>
<xml_diff>
--- a/Prototypes/iPasXLDataLayer/iPasXLDataLayer/iPasXL.12345_000.API.xlsx
+++ b/Prototypes/iPasXLDataLayer/iPasXLDataLayer/iPasXL.12345_000.API.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Tag</t>
   </si>
@@ -51,40 +51,37 @@
     <t>Equip-002</t>
   </si>
   <si>
+    <t>PT-8</t>
+  </si>
+  <si>
+    <t>PDT-8</t>
+  </si>
+  <si>
+    <t>DESC-9</t>
+  </si>
+  <si>
+    <t>PDT-3</t>
+  </si>
+  <si>
+    <t>DESC-3</t>
+  </si>
+  <si>
+    <t>PT-7</t>
+  </si>
+  <si>
+    <t>PDT-9</t>
+  </si>
+  <si>
     <t>Equip-003</t>
   </si>
   <si>
+    <t>DESC-2</t>
+  </si>
+  <si>
     <t>Equip-004</t>
   </si>
   <si>
-    <t>PT-6</t>
-  </si>
-  <si>
-    <t>PDT-6</t>
-  </si>
-  <si>
-    <t>DESC-5</t>
-  </si>
-  <si>
     <t>PT-3</t>
-  </si>
-  <si>
-    <t>PT-8</t>
-  </si>
-  <si>
-    <t>PDT-4</t>
-  </si>
-  <si>
-    <t>DESC-6</t>
-  </si>
-  <si>
-    <t>PDT-8</t>
-  </si>
-  <si>
-    <t>DESC-2</t>
-  </si>
-  <si>
-    <t>PDT-9</t>
   </si>
 </sst>
 </file>
@@ -419,7 +416,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,28 +466,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -501,83 +498,83 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
       <c r="I4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
       <c r="I5">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Generic Excel DataLayer (iPasXL) missed two files
</commit_message>
<xml_diff>
--- a/Prototypes/iPasXLDataLayer/iPasXLDataLayer/iPasXL.12345_000.API.xlsx
+++ b/Prototypes/iPasXLDataLayer/iPasXLDataLayer/iPasXL.12345_000.API.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Tag</t>
   </si>
@@ -51,37 +51,40 @@
     <t>Equip-002</t>
   </si>
   <si>
-    <t>PT-8</t>
-  </si>
-  <si>
-    <t>PDT-8</t>
-  </si>
-  <si>
-    <t>DESC-9</t>
-  </si>
-  <si>
-    <t>PDT-3</t>
-  </si>
-  <si>
-    <t>DESC-3</t>
-  </si>
-  <si>
-    <t>PT-7</t>
-  </si>
-  <si>
-    <t>PDT-9</t>
-  </si>
-  <si>
     <t>Equip-003</t>
   </si>
   <si>
-    <t>DESC-2</t>
-  </si>
-  <si>
     <t>Equip-004</t>
   </si>
   <si>
-    <t>PT-3</t>
+    <t>DESC-8</t>
+  </si>
+  <si>
+    <t>PT-4</t>
+  </si>
+  <si>
+    <t>PDT-5</t>
+  </si>
+  <si>
+    <t>DESC-5</t>
+  </si>
+  <si>
+    <t>PT-2</t>
+  </si>
+  <si>
+    <t>PDT-4</t>
+  </si>
+  <si>
+    <t>DESC-6</t>
+  </si>
+  <si>
+    <t>PT-6</t>
+  </si>
+  <si>
+    <t>DESC-7</t>
+  </si>
+  <si>
+    <t>PT-5</t>
   </si>
 </sst>
 </file>
@@ -469,25 +472,25 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>4</v>
       </c>
       <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>6</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
       <c r="H2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -495,86 +498,86 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
         <v>7</v>
-      </c>
-      <c r="I3">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>7</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I4">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>